<commit_message>
Computer players now have the ability to make random moves
</commit_message>
<xml_diff>
--- a/artifacts/sprint-4-logs.xlsx
+++ b/artifacts/sprint-4-logs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jbens\dev\sosgame\artifacts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{111FF6EA-EFF4-414F-8272-8D1D82E77FA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A586E586-E502-4E23-BAFA-332BE73D2D8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7320" yWindow="45" windowWidth="21600" windowHeight="11190" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="2" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="User Stories" sheetId="1" r:id="rId1"/>
@@ -2669,8 +2669,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C2:G13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2877,7 +2877,7 @@
   <dimension ref="B2:H48"/>
   <sheetViews>
     <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3913,8 +3913,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BDFD0F4-363F-419F-B294-A046D2B416F4}">
   <dimension ref="B4:I30"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView topLeftCell="A24" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5170,7 +5170,7 @@
   <dimension ref="B3:G26"/>
   <sheetViews>
     <sheetView topLeftCell="A21" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F26" sqref="B4:G26"/>
+      <selection activeCell="E44" sqref="E44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5615,7 +5615,7 @@
   <dimension ref="B2:F28"/>
   <sheetViews>
     <sheetView topLeftCell="A14" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E20" sqref="B3:F28"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6099,8 +6099,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D749AFF6-9F01-4083-8483-60452F81DBFD}">
   <dimension ref="A1:L513"/>
   <sheetViews>
-    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="F58" sqref="F58"/>
+    <sheetView tabSelected="1" topLeftCell="A366" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="L389" sqref="L389"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Production code written for computer player making moves in simple game and general game. Highly inefficient
</commit_message>
<xml_diff>
--- a/artifacts/sprint-4-logs.xlsx
+++ b/artifacts/sprint-4-logs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jbens\dev\sosgame\artifacts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A586E586-E502-4E23-BAFA-332BE73D2D8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F3794E9-A632-4C14-89AA-CBDCF5051115}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="2" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="User Stories" sheetId="1" r:id="rId1"/>
@@ -1346,19 +1346,19 @@
     <t>Computer makes a move on a nonempty board in a simple game or general game when there is no opportunity to complete an SOS</t>
   </si>
   <si>
-    <t>Given an SOS application during a simple or general game on a nonempty board, when there is no opportunity to complete an SOS, then…flip a fair coin to decide whether to either make a move that does not create an opportunity to complete a SOS on the next turn or make a move that does create the opportunity to complete a SOS on the next turn...and then make the move accordingly</t>
-  </si>
-  <si>
-    <t>Given an SOS application during a simple game, when there is an opportunity to complete an SOS, then…flip a fair coin to decide whether to either complete a SOS to win the game or to make a move that does not complete the SOS…and then make the move accordingly</t>
-  </si>
-  <si>
-    <t>Given an SOS application during a general game, when there is an opportunity to complete only one SOS, then…flip a fair coin to decide whether complete the SOS or to make a move that does not complete an SOS…and then make the move accordingly</t>
-  </si>
-  <si>
-    <t>Given an SOS application during a general game, when there are multiple opportunities to complete an SOS, then choose at random from the possible moves that complete an SOS and make the corresponding move</t>
-  </si>
-  <si>
     <t>Computer makes a move when there are multiple opportunities to complete an SOS in a general game</t>
+  </si>
+  <si>
+    <t>Given an SOS application during a simple or general game on a nonempty board, when there is no opportunity to complete an SOS, then make a move on a random cell</t>
+  </si>
+  <si>
+    <t>Given an SOS application during a simple game, when there is an opportunity to complete an SOS, then…flip a fair coin to decide whether to either complete a SOS to win the game or to make a random move</t>
+  </si>
+  <si>
+    <t>Given an SOS application during a general game, when there is an opportunity to complete only one SOS, then flip a fair coin to decide whether to complete the SOS or make a random move</t>
+  </si>
+  <si>
+    <t>Given an SOS application during a general game, when there are multiple opportunities to complete an SOS, then choose at random from the possible moves that complete an SOS</t>
   </si>
 </sst>
 </file>
@@ -2670,7 +2670,7 @@
   <dimension ref="C2:G13"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2876,8 +2876,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DCE3E03-8907-42B0-9BAE-1522C8D2D080}">
   <dimension ref="B2:H48"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="E35" sqref="E35"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3433,7 +3433,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="34" spans="2:7" ht="120" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:7" ht="90" x14ac:dyDescent="0.25">
       <c r="B34" s="10"/>
       <c r="C34" s="11"/>
       <c r="D34" s="11">
@@ -3443,13 +3443,13 @@
         <v>406</v>
       </c>
       <c r="F34" s="11" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="G34" s="10" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="35" spans="2:7" ht="90" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:7" ht="75" x14ac:dyDescent="0.25">
       <c r="B35" s="10"/>
       <c r="C35" s="11"/>
       <c r="D35" s="11">
@@ -3459,13 +3459,13 @@
         <v>402</v>
       </c>
       <c r="F35" s="11" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="G35" s="10" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="36" spans="2:7" ht="90" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:7" ht="75" x14ac:dyDescent="0.25">
       <c r="B36" s="10"/>
       <c r="C36" s="11"/>
       <c r="D36" s="11">
@@ -3475,7 +3475,7 @@
         <v>403</v>
       </c>
       <c r="F36" s="11" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="G36" s="10" t="s">
         <v>17</v>
@@ -3488,10 +3488,10 @@
         <v>8.5</v>
       </c>
       <c r="E37" s="11" t="s">
+        <v>407</v>
+      </c>
+      <c r="F37" s="11" t="s">
         <v>411</v>
-      </c>
-      <c r="F37" s="11" t="s">
-        <v>410</v>
       </c>
       <c r="G37" s="10" t="s">
         <v>17</v>
@@ -6099,7 +6099,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D749AFF6-9F01-4083-8483-60452F81DBFD}">
   <dimension ref="A1:L513"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A366" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+    <sheetView topLeftCell="A366" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <selection activeCell="L389" sqref="L389"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Production code written for computer making moves in simple and general game according to acceptance criteria
</commit_message>
<xml_diff>
--- a/artifacts/sprint-4-logs.xlsx
+++ b/artifacts/sprint-4-logs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jbens\dev\sosgame\artifacts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F3794E9-A632-4C14-89AA-CBDCF5051115}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62FD2B85-ABFF-4C45-9050-AD3C816416C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="2" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="User Stories" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="920" uniqueCount="412">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="923" uniqueCount="414">
   <si>
     <t>ID</t>
   </si>
@@ -1359,6 +1359,12 @@
   </si>
   <si>
     <t>Given an SOS application during a general game, when there are multiple opportunities to complete an SOS, then choose at random from the possible moves that complete an SOS</t>
+  </si>
+  <si>
+    <t>Game board not accessible when it is red turn and red is computer</t>
+  </si>
+  <si>
+    <t>Game board not accessible when it is blue turn and blue is computer</t>
   </si>
 </sst>
 </file>
@@ -2876,8 +2882,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DCE3E03-8907-42B0-9BAE-1522C8D2D080}">
   <dimension ref="B2:H48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="F38" sqref="F38"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="H37" sqref="H37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6099,8 +6105,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D749AFF6-9F01-4083-8483-60452F81DBFD}">
   <dimension ref="A1:L513"/>
   <sheetViews>
-    <sheetView topLeftCell="A366" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="L389" sqref="L389"/>
+    <sheetView tabSelected="1" topLeftCell="A293" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H305" sqref="H305"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16417,9 +16423,11 @@
         <v>0</v>
       </c>
       <c r="K300" s="13">
-        <v>1</v>
-      </c>
-      <c r="L300" s="13"/>
+        <v>0</v>
+      </c>
+      <c r="L300" s="13" t="s">
+        <v>413</v>
+      </c>
     </row>
     <row r="301" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A301" s="13"/>
@@ -16451,7 +16459,7 @@
         <v>1</v>
       </c>
       <c r="K301" s="13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L301" s="13"/>
     </row>
@@ -16519,9 +16527,11 @@
         <v>1</v>
       </c>
       <c r="K303" s="13">
-        <v>1</v>
-      </c>
-      <c r="L303" s="13"/>
+        <v>0</v>
+      </c>
+      <c r="L303" s="13" t="s">
+        <v>412</v>
+      </c>
     </row>
     <row r="304" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A304" s="13"/>
@@ -16587,9 +16597,11 @@
         <v>1</v>
       </c>
       <c r="K305" s="13">
-        <v>1</v>
-      </c>
-      <c r="L305" s="13"/>
+        <v>0</v>
+      </c>
+      <c r="L305" s="13" t="s">
+        <v>412</v>
+      </c>
     </row>
     <row r="306" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A306" s="13"/>

</xml_diff>